<commit_message>
CCRU CCH Integration KPIs fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Small - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Small - REG.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Convenience Small'!$A$1:$AM$168</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Convenience Small'!$A$1:$AM$168</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AM$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AM$168</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2249,54 +2250,53 @@
   </sheetPr>
   <dimension ref="A1:AO168"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="S154" activeCellId="0" sqref="S154:S168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6558704453441"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8947368421053"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.8866396761134"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.1255060728745"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.2753036437247"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="62.8016194331984"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="34.2793522267206"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.9311740890688"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="90.9595141700405"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="24.1174089068826"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="131.113360323887"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="58.0283400809717"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.5465587044534"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="27.663967611336"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.3805668016194"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.3441295546559"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.7692307692308"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="63.3076923076923"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="91.8016194331984"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="132.291497975709"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="66.2267206477733"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="23.5101214574899"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.44939271255061"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="9.91093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.46153846153846"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="9.63967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14637,10 +14637,10 @@
       <c r="O154" s="6"/>
       <c r="P154" s="6"/>
       <c r="Q154" s="6"/>
-      <c r="R154" s="6"/>
-      <c r="S154" s="6" t="s">
+      <c r="R154" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S154" s="6"/>
       <c r="T154" s="6"/>
       <c r="U154" s="6"/>
       <c r="V154" s="6"/>
@@ -14702,10 +14702,10 @@
       <c r="O155" s="6"/>
       <c r="P155" s="6"/>
       <c r="Q155" s="6"/>
-      <c r="R155" s="6"/>
-      <c r="S155" s="6" t="s">
+      <c r="R155" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S155" s="6"/>
       <c r="T155" s="6"/>
       <c r="U155" s="6"/>
       <c r="V155" s="6"/>
@@ -14771,10 +14771,10 @@
       <c r="O156" s="6"/>
       <c r="P156" s="6"/>
       <c r="Q156" s="6"/>
-      <c r="R156" s="6"/>
-      <c r="S156" s="6" t="s">
+      <c r="R156" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S156" s="6"/>
       <c r="T156" s="6"/>
       <c r="U156" s="6"/>
       <c r="V156" s="6"/>
@@ -14840,10 +14840,10 @@
       <c r="O157" s="6"/>
       <c r="P157" s="6"/>
       <c r="Q157" s="6"/>
-      <c r="R157" s="6"/>
-      <c r="S157" s="6" t="s">
+      <c r="R157" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S157" s="6"/>
       <c r="T157" s="6"/>
       <c r="U157" s="6"/>
       <c r="V157" s="6"/>
@@ -14909,10 +14909,10 @@
       <c r="O158" s="6"/>
       <c r="P158" s="6"/>
       <c r="Q158" s="6"/>
-      <c r="R158" s="6"/>
-      <c r="S158" s="6" t="s">
+      <c r="R158" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S158" s="6"/>
       <c r="T158" s="6"/>
       <c r="U158" s="6"/>
       <c r="V158" s="6"/>
@@ -14978,10 +14978,10 @@
       <c r="O159" s="6"/>
       <c r="P159" s="6"/>
       <c r="Q159" s="6"/>
-      <c r="R159" s="6"/>
-      <c r="S159" s="6" t="s">
+      <c r="R159" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S159" s="6"/>
       <c r="T159" s="6"/>
       <c r="U159" s="6"/>
       <c r="V159" s="6"/>
@@ -15043,10 +15043,10 @@
       <c r="O160" s="6"/>
       <c r="P160" s="6"/>
       <c r="Q160" s="6"/>
-      <c r="R160" s="6"/>
-      <c r="S160" s="6" t="s">
+      <c r="R160" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S160" s="6"/>
       <c r="T160" s="6"/>
       <c r="U160" s="6"/>
       <c r="V160" s="6"/>
@@ -15108,10 +15108,10 @@
       <c r="O161" s="6"/>
       <c r="P161" s="6"/>
       <c r="Q161" s="6"/>
-      <c r="R161" s="6"/>
-      <c r="S161" s="6" t="s">
+      <c r="R161" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S161" s="6"/>
       <c r="T161" s="6"/>
       <c r="U161" s="6"/>
       <c r="V161" s="6"/>
@@ -15175,10 +15175,10 @@
       <c r="O162" s="6"/>
       <c r="P162" s="6"/>
       <c r="Q162" s="6"/>
-      <c r="R162" s="6"/>
-      <c r="S162" s="6" t="s">
+      <c r="R162" s="6" t="s">
         <v>559</v>
       </c>
+      <c r="S162" s="6"/>
       <c r="T162" s="6"/>
       <c r="U162" s="6"/>
       <c r="V162" s="6"/>
@@ -15242,10 +15242,10 @@
       <c r="O163" s="6"/>
       <c r="P163" s="6"/>
       <c r="Q163" s="6"/>
-      <c r="R163" s="6"/>
-      <c r="S163" s="6" t="s">
+      <c r="R163" s="6" t="s">
         <v>559</v>
       </c>
+      <c r="S163" s="6"/>
       <c r="T163" s="6"/>
       <c r="U163" s="6"/>
       <c r="V163" s="6"/>
@@ -15311,10 +15311,10 @@
       <c r="O164" s="6"/>
       <c r="P164" s="6"/>
       <c r="Q164" s="6"/>
-      <c r="R164" s="6"/>
-      <c r="S164" s="6" t="s">
+      <c r="R164" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S164" s="6"/>
       <c r="T164" s="6"/>
       <c r="U164" s="6"/>
       <c r="V164" s="6"/>
@@ -15380,10 +15380,10 @@
       <c r="O165" s="6"/>
       <c r="P165" s="6"/>
       <c r="Q165" s="6"/>
-      <c r="R165" s="6"/>
-      <c r="S165" s="6" t="s">
+      <c r="R165" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S165" s="6"/>
       <c r="T165" s="6"/>
       <c r="U165" s="6"/>
       <c r="V165" s="6"/>
@@ -15449,10 +15449,10 @@
       <c r="O166" s="6"/>
       <c r="P166" s="6"/>
       <c r="Q166" s="6"/>
-      <c r="R166" s="6"/>
-      <c r="S166" s="6" t="s">
+      <c r="R166" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S166" s="6"/>
       <c r="T166" s="6"/>
       <c r="U166" s="6"/>
       <c r="V166" s="6"/>
@@ -15518,10 +15518,10 @@
       <c r="O167" s="6"/>
       <c r="P167" s="6"/>
       <c r="Q167" s="6"/>
-      <c r="R167" s="6"/>
-      <c r="S167" s="6" t="s">
+      <c r="R167" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S167" s="6"/>
       <c r="T167" s="6"/>
       <c r="U167" s="6"/>
       <c r="V167" s="6"/>
@@ -15581,10 +15581,10 @@
       <c r="O168" s="6"/>
       <c r="P168" s="6"/>
       <c r="Q168" s="6"/>
-      <c r="R168" s="6"/>
-      <c r="S168" s="6" t="s">
+      <c r="R168" s="6" t="s">
         <v>530</v>
       </c>
+      <c r="S168" s="6"/>
       <c r="T168" s="6"/>
       <c r="U168" s="6"/>
       <c r="V168" s="6"/>

</xml_diff>